<commit_message>
add CLI interface and datetime support
</commit_message>
<xml_diff>
--- a/bentry/example.xlsx
+++ b/bentry/example.xlsx
@@ -2,16 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,34 +19,110 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t>Apples</t>
-  </si>
-  <si>
-    <t>Cheeries</t>
-  </si>
-  <si>
-    <t>Pears</t>
-  </si>
-  <si>
-    <t>Oranges</t>
-  </si>
-  <si>
-    <t>Bananas</t>
-  </si>
-  <si>
-    <t>Strawberries</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="19">
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>alotted</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>remaining</t>
+  </si>
+  <si>
+    <t>Day-by-day</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>legal pads</t>
+  </si>
+  <si>
+    <t>uber</t>
+  </si>
+  <si>
+    <t>groceries</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>lunch</t>
+  </si>
+  <si>
+    <t>dinner</t>
+  </si>
+  <si>
+    <t>movie rental</t>
+  </si>
+  <si>
+    <t>bus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -62,7 +136,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,15 +144,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,127 +509,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1">
-        <v>42830</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="5">
+        <v>42931</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>42830</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>42831</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="3">
+        <f>540/4</f>
+        <v>135</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>50</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>15</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
+        <f>SUM(C9:C22)</f>
+        <v>126.07000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3">
+        <f>SUM(G9:G15)</f>
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="3">
+        <f>SUM(K9:K16)</f>
+        <v>21.23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="3">
+        <f>SUM(O9:O10)</f>
+        <v>8.3699999999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <f>C3-C4</f>
+        <v>8.9299999999999926</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3">
+        <f>G3-G4</f>
+        <v>47</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="3">
+        <f>K3-K4</f>
+        <v>-6.23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="3">
+        <f>O3-O4</f>
+        <v>11.63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17" customHeight="1" thickBot="1">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="E7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="I7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="M7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" ht="16" customHeight="1" thickTop="1">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="4">
+        <v>42925</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3">
+        <v>25.35</v>
+      </c>
+      <c r="E9" s="4">
+        <v>42926</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="I9" s="4">
+        <v>42927</v>
+      </c>
+      <c r="J9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M9" s="4">
+        <v>42927</v>
+      </c>
+      <c r="N9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="3">
+        <v>8.3699999999999992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="4">
+        <v>42925</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>42833</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>42835</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>42835</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>42835</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>98</v>
-      </c>
+      <c r="C10" s="3">
+        <v>2.85</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="4">
+        <v>42928</v>
+      </c>
+      <c r="J10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="4">
+        <v>42925</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2.78</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="4">
+        <v>42929</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="3">
+        <f>2.5+1.25</f>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="4">
+        <v>42925</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3">
+        <v>9.58</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="4">
+        <v>42930</v>
+      </c>
+      <c r="J12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1">
+        <v>42929</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3">
+        <v>7.98</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="4">
+        <v>42928</v>
+      </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="3">
+        <v>9.98</v>
+      </c>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="4">
+        <v>42929</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3">
+        <v>9.61</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="4"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="4">
+        <v>42930</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3">
+        <v>58.31</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="G15" s="3"/>
+      <c r="I15" s="4"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="4">
+        <v>42930</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3">
+        <v>9.61</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="1"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="1"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="1"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="4"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="N23" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="M7:O7"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>